<commit_message>
Applied WidgetTable by Using Pandas, add,del,save button ok, test copy.py
</commit_message>
<xml_diff>
--- a/data/test2.xlsx
+++ b/data/test2.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\코린이\04. 개인 프로젝트\01.angle_price\자료\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848B76A0-135F-4390-92DC-A06E504ECEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="b" sheetId="1" r:id="rId1"/>
+    <sheet name="AABC" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,12 +43,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -62,15 +56,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -116,23 +103,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -174,7 +153,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,27 +185,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,24 +219,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,16 +394,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -485,7 +426,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -499,7 +440,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -513,7 +454,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -527,7 +468,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -541,9 +482,20 @@
         <v>2100</v>
       </c>
     </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>1.7</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>